<commit_message>
Updated the Nayar Template. Made changes to KPI tool box.
</commit_message>
<xml_diff>
--- a/Projects/CCNAYARMX/Fondas/Data/Nayar Comidas Fondas Template_v2.xlsx
+++ b/Projects/CCNAYARMX/Fondas/Data/Nayar Comidas Fondas Template_v2.xlsx
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$G$58</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$G$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$G$58</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$G$57</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$G$57</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$1:$G$57</definedName>
@@ -28,6 +28,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$G$57</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$G$57</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$G$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$G$57</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="225">
   <si>
     <t xml:space="preserve">KPI Number</t>
   </si>
@@ -896,7 +897,7 @@
     <t xml:space="preserve">product_type</t>
   </si>
   <si>
-    <t xml:space="preserve">product_short_name</t>
+    <t xml:space="preserve">product_fk</t>
   </si>
   <si>
     <t xml:space="preserve">Numerator Entity</t>
@@ -926,7 +927,7 @@
     <t xml:space="preserve">POS</t>
   </si>
   <si>
-    <t xml:space="preserve">Comunicacion Marca,Coca-Cola POS Other</t>
+    <t xml:space="preserve">2804,2357</t>
   </si>
   <si>
     <t xml:space="preserve">manufacturer_fk</t>
@@ -941,15 +942,9 @@
     <t xml:space="preserve">100/0</t>
   </si>
   <si>
-    <t xml:space="preserve">Comunicacion Paquete</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comunicación Interior</t>
   </si>
   <si>
-    <t xml:space="preserve">Comunicacion Marca</t>
-  </si>
-  <si>
     <t xml:space="preserve">Task/ Template Group</t>
   </si>
   <si>
@@ -1077,9 +1072,6 @@
   </si>
   <si>
     <t xml:space="preserve">Assortment1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_fk</t>
   </si>
   <si>
     <t xml:space="preserve">sub_category_fk</t>
@@ -1706,25 +1698,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="L5 D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.8851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="72.7111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="81.6296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.862962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="74.5740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="83.6851851851852"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,7 +1742,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
@@ -1773,7 +1765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="34" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
@@ -1819,7 +1811,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
@@ -1840,7 +1832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
@@ -1861,7 +1853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>21</v>
@@ -1874,7 +1866,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
@@ -1895,7 +1887,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>7</v>
       </c>
@@ -1916,7 +1908,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
@@ -1937,7 +1929,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
@@ -1958,7 +1950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>10</v>
       </c>
@@ -1979,7 +1971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="6" t="s">
         <v>33</v>
@@ -1992,7 +1984,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>11</v>
       </c>
@@ -2013,7 +2005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>12</v>
       </c>
@@ -2034,7 +2026,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>13</v>
       </c>
@@ -2055,7 +2047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>14</v>
       </c>
@@ -2076,7 +2068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>15</v>
       </c>
@@ -2097,7 +2089,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="6" t="s">
         <v>43</v>
@@ -2110,7 +2102,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>16</v>
       </c>
@@ -2131,7 +2123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>17</v>
       </c>
@@ -2152,7 +2144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>18</v>
       </c>
@@ -2173,7 +2165,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <v>19</v>
       </c>
@@ -2194,7 +2186,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
         <v>20</v>
       </c>
@@ -2215,7 +2207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="6" t="s">
         <v>53</v>
@@ -2228,7 +2220,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>21</v>
       </c>
@@ -2249,7 +2241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>22</v>
       </c>
@@ -2270,7 +2262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>23</v>
       </c>
@@ -2291,7 +2283,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>24</v>
       </c>
@@ -2312,7 +2304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
         <v>25</v>
       </c>
@@ -2333,7 +2325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="6" t="s">
         <v>63</v>
@@ -2346,7 +2338,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>26</v>
       </c>
@@ -2367,7 +2359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>27</v>
       </c>
@@ -2388,7 +2380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="n">
         <v>28</v>
       </c>
@@ -2409,7 +2401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="6" t="s">
         <v>69</v>
@@ -2422,7 +2414,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>29</v>
       </c>
@@ -2443,7 +2435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>30</v>
       </c>
@@ -2464,7 +2456,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="n">
         <v>31</v>
       </c>
@@ -2485,7 +2477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="6" t="s">
         <v>75</v>
@@ -2498,7 +2490,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <v>32</v>
       </c>
@@ -2519,7 +2511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>33</v>
       </c>
@@ -2540,7 +2532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="n">
         <v>34</v>
       </c>
@@ -2561,7 +2553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="6" t="s">
         <v>81</v>
@@ -2574,7 +2566,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
         <v>35</v>
       </c>
@@ -2595,7 +2587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
         <v>36</v>
       </c>
@@ -2616,7 +2608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
         <v>37</v>
       </c>
@@ -2637,7 +2629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
         <v>38</v>
       </c>
@@ -2658,7 +2650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="n">
         <v>39</v>
       </c>
@@ -2679,7 +2671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="17" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
         <v>40</v>
       </c>
@@ -2702,7 +2694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="17" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
         <v>41</v>
       </c>
@@ -2725,7 +2717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="17" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
         <v>42</v>
       </c>
@@ -2748,7 +2740,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="17" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
         <v>43</v>
       </c>
@@ -2771,7 +2763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="34" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
         <v>44</v>
       </c>
@@ -2792,7 +2784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="34" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
         <v>45</v>
       </c>
@@ -2813,7 +2805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="34" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
         <v>46</v>
       </c>
@@ -2834,7 +2826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="17" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="n">
         <v>47</v>
       </c>
@@ -2855,7 +2847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="n">
         <v>48</v>
       </c>
@@ -2876,7 +2868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="16" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="n">
         <v>49</v>
       </c>
@@ -2896,7 +2888,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G58"/>
+  <autoFilter ref="A1:G58">
+    <filterColumn colId="3">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Respeto-Fondas-Rsr"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2915,24 +2913,25 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.8444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="80.0592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3148148148148"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="31.7518518518519"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.8037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.8444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.4481481481482"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="82.1185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.437037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="51.6740740740741"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.2259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3023,7 +3022,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>41</v>
       </c>
@@ -3048,8 +3047,8 @@
       <c r="H3" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>126</v>
+      <c r="I3" s="12" t="n">
+        <v>2805</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>122</v>
@@ -3064,7 +3063,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>42</v>
       </c>
@@ -3081,7 +3080,7 @@
         <v>118</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>11</v>
@@ -3089,8 +3088,8 @@
       <c r="H4" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>128</v>
+      <c r="I4" s="12" t="n">
+        <v>2804</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>122</v>
@@ -3122,7 +3121,7 @@
         <v>118</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>11</v>
@@ -3130,8 +3129,8 @@
       <c r="H5" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>126</v>
+      <c r="I5" s="12" t="n">
+        <v>2805</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>122</v>
@@ -3164,27 +3163,27 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="L5 B24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.9592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.5925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="69.8703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.9518518518519"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.6888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.4740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.6333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.4407407407407"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3201,7 +3200,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>108</v>
@@ -3213,16 +3212,16 @@
         <v>6</v>
       </c>
       <c r="I1" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>112</v>
@@ -3231,7 +3230,7 @@
         <v>114</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P1" s="10" t="s">
         <v>116</v>
@@ -3251,22 +3250,22 @@
         <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>139</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>122</v>
@@ -3299,22 +3298,22 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="1" sqref="L5 Q2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.9703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="31.062962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="67.0296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.8111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.637037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="31.8481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="68.6925925925926"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.4962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3331,28 +3330,28 @@
         <v>5</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="J1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>140</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>142</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>112</v>
@@ -3361,7 +3360,7 @@
         <v>114</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>116</v>
@@ -3384,19 +3383,19 @@
         <v>14</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J2" s="20"/>
       <c r="K2" s="19"/>
@@ -3408,10 +3407,10 @@
         <v>123</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Q2" s="21" t="s">
         <v>125</v>
@@ -3435,21 +3434,21 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="L5 C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.1074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.7148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="140.22962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="74.7703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.3814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="143.755555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="76.7296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3469,13 +3468,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>148</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>116</v>
@@ -3486,7 +3485,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>8</v>
@@ -3498,7 +3497,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>9</v>
@@ -3515,7 +3514,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>102</v>
@@ -3527,10 +3526,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>14</v>
@@ -3544,7 +3543,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>104</v>
@@ -3556,10 +3555,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>15</v>
@@ -3573,7 +3572,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>106</v>
@@ -3585,10 +3584,10 @@
         <v>10</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>16</v>
@@ -3615,20 +3614,20 @@
   </sheetPr>
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="1" sqref="L5 O1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.3555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.8703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.4111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.6333333333333"/>
     <col collapsed="false" hidden="true" max="10" min="5" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3648,34 +3647,34 @@
         <v>5</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>108</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>163</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>165</v>
       </c>
       <c r="P1" s="26" t="s">
         <v>112</v>
@@ -3713,41 +3712,41 @@
         <v>26</v>
       </c>
       <c r="F2" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="K2" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="J2" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="K2" s="30" t="s">
-        <v>170</v>
-      </c>
       <c r="L2" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M2" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P2" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q2" s="29"/>
       <c r="R2" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S2" s="29"/>
       <c r="T2" s="2" t="s">
@@ -3774,41 +3773,41 @@
         <v>26</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
@@ -3835,41 +3834,41 @@
         <v>26</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I4" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>169</v>
-      </c>
       <c r="K4" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P4" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
@@ -3896,41 +3895,41 @@
         <v>26</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K5" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L5" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M5" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P5" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2" t="s">
@@ -3957,41 +3956,41 @@
         <v>26</v>
       </c>
       <c r="F6" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="J6" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="K6" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="J6" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>170</v>
-      </c>
       <c r="L6" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2" t="s">
@@ -4018,41 +4017,41 @@
         <v>26</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J7" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K7" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L7" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M7" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P7" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2" t="s">
@@ -4079,41 +4078,41 @@
         <v>26</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="J8" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I8" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>169</v>
-      </c>
       <c r="K8" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L8" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M8" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2" t="s">
@@ -4140,41 +4139,41 @@
         <v>26</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K9" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L9" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2" t="s">
@@ -4201,41 +4200,41 @@
         <v>26</v>
       </c>
       <c r="F10" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I10" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="J10" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I10" s="29" t="s">
+      <c r="K10" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="J10" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>170</v>
-      </c>
       <c r="L10" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M10" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2" t="s">
@@ -4262,41 +4261,41 @@
         <v>26</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K11" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L11" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M11" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P11" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2" t="s">
@@ -4323,41 +4322,41 @@
         <v>26</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="J12" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I12" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>169</v>
-      </c>
       <c r="K12" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M12" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P12" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="2" t="s">
@@ -4384,41 +4383,41 @@
         <v>26</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K13" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L13" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M13" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P13" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2" t="s">
@@ -4445,41 +4444,41 @@
         <v>26</v>
       </c>
       <c r="F14" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I14" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="J14" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="K14" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="J14" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="K14" s="30" t="s">
-        <v>170</v>
-      </c>
       <c r="L14" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M14" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P14" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="2" t="s">
@@ -4506,41 +4505,41 @@
         <v>26</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K15" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L15" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M15" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P15" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="2" t="s">
@@ -4567,41 +4566,41 @@
         <v>26</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I16" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="J16" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I16" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="J16" s="30" t="s">
-        <v>169</v>
-      </c>
       <c r="K16" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L16" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M16" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P16" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="2" t="s">
@@ -4628,41 +4627,41 @@
         <v>26</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K17" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M17" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P17" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="2" t="s">
@@ -4689,41 +4688,41 @@
         <v>26</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I18" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>169</v>
-      </c>
       <c r="K18" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L18" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M18" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P18" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="2" t="s">
@@ -4750,41 +4749,41 @@
         <v>26</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J19" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K19" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L19" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M19" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P19" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S19" s="2"/>
       <c r="T19" s="2" t="s">
@@ -4811,41 +4810,41 @@
         <v>26</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I20" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="J20" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I20" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="J20" s="30" t="s">
-        <v>169</v>
-      </c>
       <c r="K20" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M20" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N20" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P20" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="2" t="s">
@@ -4872,41 +4871,41 @@
         <v>26</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K21" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L21" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M21" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N21" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="2" t="s">
@@ -4933,41 +4932,41 @@
         <v>26</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="J22" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="I22" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="J22" s="30" t="s">
-        <v>169</v>
-      </c>
       <c r="K22" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L22" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M22" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P22" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="2" t="s">
@@ -4994,41 +4993,41 @@
         <v>26</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J23" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K23" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L23" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M23" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P23" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="2" t="s">
@@ -5055,41 +5054,41 @@
         <v>26</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J24" s="30" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K24" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L24" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M24" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N24" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P24" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="2" t="s">
@@ -5116,41 +5115,41 @@
         <v>26</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J25" s="30" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L25" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M25" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N25" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S25" s="2"/>
       <c r="T25" s="2" t="s">
@@ -5177,41 +5176,41 @@
         <v>26</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J26" s="30" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K26" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L26" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M26" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N26" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P26" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="2" t="s">
@@ -5238,41 +5237,41 @@
         <v>26</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J27" s="30" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K27" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L27" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M27" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N27" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P27" s="20" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="2" t="s">
@@ -5300,17 +5299,17 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D6" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="L5 D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="122.003703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="161.003703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="160.611111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="125.137037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="165.118518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="164.725925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5318,13 +5317,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5332,13 +5331,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5346,13 +5345,13 @@
         <v>33</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5360,13 +5359,13 @@
         <v>43</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5374,13 +5373,13 @@
         <v>53</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5388,13 +5387,13 @@
         <v>81</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5402,10 +5401,10 @@
         <v>63</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D7" s="33"/>
     </row>
@@ -5414,10 +5413,10 @@
         <v>69</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D8" s="33"/>
     </row>
@@ -5426,10 +5425,10 @@
         <v>75</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D9" s="33"/>
     </row>
@@ -5451,22 +5450,22 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="L5 H9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.0222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="38.7074074074074"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.54444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.8074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.6888888888889"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.4222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5489,13 +5488,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="199.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5518,10 +5517,10 @@
         <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="199.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5544,10 +5543,10 @@
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="199.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5570,10 +5569,10 @@
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="199.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5596,10 +5595,10 @@
         <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5622,10 +5621,10 @@
         <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5648,10 +5647,10 @@
         <v>22</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5674,10 +5673,10 @@
         <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="242.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5700,13 +5699,13 @@
         <v>22</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>53</v>
       </c>
       <c r="I9" s="35" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -5727,23 +5726,23 @@
   </sheetPr>
   <dimension ref="A1:L65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="1" sqref="L5 I4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="93.6814814814815"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="55.0740740740741"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="49.6814814814815"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="66.2444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="96.1333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.4444444444444"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="50.9555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="67.9111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5766,19 +5765,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L1" s="22"/>
     </row>
@@ -5803,14 +5802,14 @@
       </c>
       <c r="G2" s="35"/>
       <c r="H2" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J2" s="38"/>
       <c r="K2" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L2" s="22"/>
     </row>
@@ -5834,17 +5833,17 @@
         <v>19</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="35" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5868,14 +5867,14 @@
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="35" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5899,14 +5898,14 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="35" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5928,14 +5927,14 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="35" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>